<commit_message>
More exploration of parameters
</commit_message>
<xml_diff>
--- a/nesh/lambda calculations.xlsx
+++ b/nesh/lambda calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nesh/Documents/Repositories/icecontinuum/nesh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A39EA8-26F1-0C44-9FDB-28573DF50357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C6CC21-4D7C-3F4B-9F02-0332A87243B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="15480" xr2:uid="{2DDA9610-AECA-0C43-BEDC-9A13351D73ED}"/>
   </bookViews>
@@ -287,7 +287,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$13</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -329,7 +329,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$13</c:f>
+              <c:f>Sheet1!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -612,66 +612,126 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$24:$A$31</c:f>
+              <c:f>Sheet1!$B$23:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.19500000000000001</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.23</c:v>
+                  <c:v>0.27500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27500000000000002</c:v>
+                  <c:v>0.23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3</c:v>
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.02</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.03</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.05</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$24:$D$31</c:f>
+              <c:f>Sheet1!$E$23:$E$40</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>9.8684210526315788</c:v>
+                  <c:v>2.7075812274368234</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.775862068965518</c:v>
+                  <c:v>4.1073384446878416</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.194029850746269</c:v>
+                  <c:v>6.1983471074380168</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.194029850746269</c:v>
+                  <c:v>8.4269662921348303</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.714285714285714</c:v>
+                  <c:v>9.1463414634146343</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.1463414634146343</c:v>
+                  <c:v>10.714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4269662921348303</c:v>
+                  <c:v>11.194029850746269</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.261261261261261</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.85383502170767</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44.117647058823529</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27.075812274368232</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.161290322580644</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.396694214876034</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.756756756756757</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.4117647058823533</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.0612244897959182</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -698,7 +758,8 @@
         <c:axId val="1158433920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.19"/>
+          <c:max val="1"/>
+          <c:min val="-0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -761,7 +822,7 @@
         <c:axId val="1158381712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="8"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1988,15 +2049,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1282700</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2025,15 +2086,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>984250</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>577850</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2358,824 +2419,1216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FACA8F-BEA8-A344-9B24-B4206D9D79F6}">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="119" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="10" max="11" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.5" customWidth="1"/>
-    <col min="13" max="13" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="11" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
+    <col min="14" max="14" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <f>E3^$B$15*B3^$B$18*J3^$B$17*H3^$B$16*10</f>
+    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B2" s="4">
+        <f>F2^$C$14*C2^$C$17*K2^$C$16*I2^$C$15*10</f>
         <v>0.32659863237109038</v>
       </c>
-      <c r="B3">
+      <c r="C2">
         <v>75</v>
       </c>
-      <c r="C3" s="4">
+      <c r="D2" s="4">
         <v>24.9</v>
       </c>
-      <c r="D3" s="5">
-        <f>B3/C3</f>
+      <c r="E2" s="5">
+        <f>C2/D2</f>
         <v>3.0120481927710845</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F2" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G2" s="3">
         <v>0.2</v>
       </c>
-      <c r="G3">
+      <c r="H2">
         <v>0.19</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I2" s="6">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I3">
+      <c r="J2">
         <v>1</v>
       </c>
+      <c r="K2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B3" s="4">
+        <f>F3^$C$14*C3^$C$17*K3^$C$16*I3^$C$15*10</f>
+        <v>0.34299717028501764</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3" s="4">
+        <v>22.9</v>
+      </c>
+      <c r="E3" s="5">
+        <f>C3/D3</f>
+        <v>3.2751091703056772</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H3">
+        <v>0.19</v>
+      </c>
+      <c r="I3" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
       <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <f>F4^$C$14*C4^$C$17*K4^$C$16*I4^$C$15*10</f>
+        <v>0.34299717028501764</v>
+      </c>
+      <c r="C4">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <f>E4^$B$15*B4^$B$18*J4^$B$17*H4^$B$16*10</f>
-        <v>0.34299717028501764</v>
-      </c>
-      <c r="B4">
+      <c r="D4" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="E4" s="5">
+        <f>C4/D4</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H4">
+        <v>0.19</v>
+      </c>
+      <c r="I4" s="6">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <f>F5^$C$14*C5^$C$17*K5^$C$16*I5^$C$15*10</f>
+        <v>0.48507125007266588</v>
+      </c>
+      <c r="C5">
         <v>75</v>
       </c>
-      <c r="C4" s="4">
-        <v>22.9</v>
-      </c>
-      <c r="D4" s="5">
-        <f>B4/C4</f>
-        <v>3.2751091703056772</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D5" s="4">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5">
+        <f>C5/D5</f>
+        <v>4.6875</v>
+      </c>
+      <c r="F5" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G5" s="3">
         <v>0.2</v>
       </c>
-      <c r="G4">
+      <c r="H5">
         <v>0.19</v>
       </c>
-      <c r="H4" s="6">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="I4">
+      <c r="I5" s="6">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="J4">
+      <c r="K5">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <f>E5^$B$15*B5^$B$18*J5^$B$17*H5^$B$16*10</f>
-        <v>0.34299717028501764</v>
-      </c>
-      <c r="B5">
+      <c r="P5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <f>F6^$C$14*C6^$C$17*K6^$C$16*I6^$C$15*10</f>
+        <v>0.48507125007266588</v>
+      </c>
+      <c r="C6">
         <v>75</v>
       </c>
-      <c r="C5" s="4">
-        <v>22.5</v>
-      </c>
-      <c r="D5" s="5">
-        <f>B5/C5</f>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="D6" s="4">
+        <v>15.4</v>
+      </c>
+      <c r="E6" s="5">
+        <f>C6/D6</f>
+        <v>4.8701298701298699</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G6" s="3">
         <v>0.2</v>
       </c>
-      <c r="G5">
+      <c r="H6">
         <v>0.19</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I6" s="6">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I5">
+      <c r="J6">
+        <v>0.5</v>
+      </c>
+      <c r="K6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <f>F7^$C$14*C7^$C$17*K7^$C$16*I7^$C$15*10</f>
+        <v>0.48507125007266588</v>
+      </c>
+      <c r="C7">
+        <v>75</v>
+      </c>
+      <c r="D7" s="4">
+        <v>14.8</v>
+      </c>
+      <c r="E7" s="5">
+        <f>C7/D7</f>
+        <v>5.0675675675675675</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H7">
+        <v>0.19</v>
+      </c>
+      <c r="I7" s="6">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J7">
+        <v>0.2</v>
+      </c>
+      <c r="K7">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <f>F8^$C$14*C8^$C$17*K8^$C$16*I8^$C$15*10</f>
+        <v>0.76696498884737041</v>
+      </c>
+      <c r="C8">
+        <v>75</v>
+      </c>
+      <c r="D8" s="4">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5">
+        <f>C8/D8</f>
+        <v>7.5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H8">
+        <v>0.19</v>
+      </c>
+      <c r="I8" s="6">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J8">
         <v>1</v>
       </c>
-      <c r="J5">
+      <c r="K8">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <f>E6^$B$15*B6^$B$18*J6^$B$17*H6^$B$16*10</f>
-        <v>0.48507125007266588</v>
-      </c>
-      <c r="B6">
+      <c r="P8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <f>F9^$C$14*C9^$C$17*K9^$C$16*I9^$C$15*10</f>
+        <v>0.76696498884737052</v>
+      </c>
+      <c r="C9">
         <v>75</v>
       </c>
-      <c r="C6" s="4">
+      <c r="D9" s="4">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E9" s="5">
+        <f>C9/D9</f>
+        <v>7.7319587628865989</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H9">
+        <v>0.19</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <f>F10^$C$14*C10^$C$17*K10^$C$16*I10^$C$15*10</f>
+        <v>0.76696498884737052</v>
+      </c>
+      <c r="C10">
+        <v>120</v>
+      </c>
+      <c r="D10" s="4">
+        <v>15.4</v>
+      </c>
+      <c r="E10" s="5">
+        <f>C10/D10</f>
+        <v>7.7922077922077921</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H10">
+        <v>0.19</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>34</v>
+      </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <f>F11^$C$14*C11^$C$17*K11^$C$16*I11^$C$15*10</f>
+        <v>1.0846522890932808</v>
+      </c>
+      <c r="C11">
+        <v>75</v>
+      </c>
+      <c r="D11" s="4">
+        <v>6.96</v>
+      </c>
+      <c r="E11" s="5">
+        <f>C11/D11</f>
+        <v>10.775862068965518</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H11">
+        <v>0.19</v>
+      </c>
+      <c r="I11" s="6">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <f>F12^$C$14*C12^$C$17*K12^$C$16*I12^$C$15*10</f>
+        <v>1.4142135623730949</v>
+      </c>
+      <c r="C12">
+        <v>75</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="E12" s="5">
+        <f>C12/D12</f>
+        <v>14.423076923076923</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H12">
+        <v>0.19</v>
+      </c>
+      <c r="I12" s="6">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5">
-        <f>B6/C6</f>
-        <v>4.6875</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <f>G23</f>
+        <v>0.9</v>
+      </c>
+      <c r="C23">
+        <v>75</v>
+      </c>
+      <c r="D23" s="4">
+        <v>27.7</v>
+      </c>
+      <c r="E23" s="5">
+        <f>C23/D23</f>
+        <v>2.7075812274368234</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="H23">
+        <v>0.19</v>
+      </c>
+      <c r="I23" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <f>G24</f>
+        <v>0.6</v>
+      </c>
+      <c r="C24">
+        <v>75</v>
+      </c>
+      <c r="D24" s="4">
+        <v>18.260000000000002</v>
+      </c>
+      <c r="E24" s="5">
+        <f>C24/D24</f>
+        <v>4.1073384446878416</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H24">
+        <v>0.19</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <f>G25</f>
+        <v>0.4</v>
+      </c>
+      <c r="C25">
+        <v>75</v>
+      </c>
+      <c r="D25" s="4">
+        <v>12.1</v>
+      </c>
+      <c r="E25" s="5">
+        <f>C25/D25</f>
+        <v>6.1983471074380168</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H25">
+        <v>0.19</v>
+      </c>
+      <c r="I25" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <f>G26</f>
+        <v>0.3</v>
+      </c>
+      <c r="C26">
+        <v>75</v>
+      </c>
+      <c r="D26" s="4">
+        <v>8.9</v>
+      </c>
+      <c r="E26" s="5">
+        <f>C26/D26</f>
+        <v>8.4269662921348303</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="H26">
+        <v>0.19</v>
+      </c>
+      <c r="I26" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <f>G27</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="C27">
+        <v>75</v>
+      </c>
+      <c r="D27" s="4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E27" s="5">
+        <f>C27/D27</f>
+        <v>9.1463414634146343</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="H27">
+        <v>0.19</v>
+      </c>
+      <c r="I27" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
+        <f>G28</f>
+        <v>0.25</v>
+      </c>
+      <c r="C28">
+        <v>75</v>
+      </c>
+      <c r="D28" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="E28" s="5">
+        <f>C28/D28</f>
+        <v>10</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H28">
+        <v>0.19</v>
+      </c>
+      <c r="I28" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
+        <f>G29</f>
+        <v>0.23</v>
+      </c>
+      <c r="C29">
+        <v>75</v>
+      </c>
+      <c r="D29" s="4">
+        <v>7</v>
+      </c>
+      <c r="E29" s="5">
+        <f>C29/D29</f>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="H29">
+        <v>0.19</v>
+      </c>
+      <c r="I29" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
+        <f>G30</f>
+        <v>0.22</v>
+      </c>
+      <c r="C30">
+        <v>75</v>
+      </c>
+      <c r="D30" s="4">
+        <v>6.7</v>
+      </c>
+      <c r="E30" s="5">
+        <f>C30/D30</f>
+        <v>11.194029850746269</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="H30">
+        <v>0.19</v>
+      </c>
+      <c r="I30" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
+        <f>G31</f>
+        <v>0.21</v>
+      </c>
+      <c r="C31">
+        <v>75</v>
+      </c>
+      <c r="D31" s="4">
+        <v>6.66</v>
+      </c>
+      <c r="E31" s="5">
+        <f>C31/D31</f>
+        <v>11.261261261261261</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="H31">
+        <v>0.19</v>
+      </c>
+      <c r="I31" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
+        <f>G32</f>
         <v>0.2</v>
       </c>
-      <c r="G6">
+      <c r="C32">
+        <v>75</v>
+      </c>
+      <c r="D32" s="4">
+        <v>6.91</v>
+      </c>
+      <c r="E32" s="5">
+        <f>C32/D32</f>
+        <v>10.85383502170767</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H32">
         <v>0.19</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I32" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I6">
+      <c r="J32">
         <v>1</v>
       </c>
-      <c r="J6">
+      <c r="K32">
         <v>34</v>
       </c>
-      <c r="O6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <f>E7^$B$15*B7^$B$18*J7^$B$17*H7^$B$16*10</f>
-        <v>0.48507125007266588</v>
-      </c>
-      <c r="B7">
+    </row>
+    <row r="33" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
+        <f>G33</f>
+        <v>-0.01</v>
+      </c>
+      <c r="C33">
         <v>75</v>
       </c>
-      <c r="C7" s="4">
-        <v>15.4</v>
-      </c>
-      <c r="D7" s="5">
-        <f>B7/C7</f>
-        <v>4.8701298701298699</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G7">
+      <c r="D33" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="E33" s="5">
+        <f>C33/D33</f>
+        <v>44.117647058823529</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G33" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="H33">
         <v>0.19</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I33" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I7">
-        <v>0.5</v>
-      </c>
-      <c r="J7">
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <f>E8^$B$15*B8^$B$18*J8^$B$17*H8^$B$16*10</f>
-        <v>0.48507125007266588</v>
-      </c>
-      <c r="B8">
+    <row r="34" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
+        <f>G34</f>
+        <v>-0.02</v>
+      </c>
+      <c r="C34">
         <v>75</v>
       </c>
-      <c r="C8" s="4">
-        <v>14.8</v>
-      </c>
-      <c r="D8" s="5">
-        <f>B8/C8</f>
-        <v>5.0675675675675675</v>
-      </c>
-      <c r="E8" s="2">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G8">
+      <c r="D34" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E34" s="5">
+        <f>C34/D34</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G34" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="H34">
         <v>0.19</v>
       </c>
-      <c r="H8" s="6">
+      <c r="I34" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I8">
-        <v>0.2</v>
-      </c>
-      <c r="J8">
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
         <v>34</v>
       </c>
-      <c r="L8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <f>E9^$B$15*B9^$B$18*J9^$B$17*H9^$B$16*10</f>
-        <v>0.76696498884737041</v>
-      </c>
-      <c r="B9">
+    </row>
+    <row r="35" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
+        <f>G35</f>
+        <v>-0.03</v>
+      </c>
+      <c r="C35">
         <v>75</v>
       </c>
-      <c r="C9" s="4">
-        <v>10</v>
-      </c>
-      <c r="D9" s="5">
-        <f>B9/C9</f>
-        <v>7.5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G9">
+      <c r="D35" s="4">
+        <v>2.77</v>
+      </c>
+      <c r="E35" s="5">
+        <f>C35/D35</f>
+        <v>27.075812274368232</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G35" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="H35">
         <v>0.19</v>
       </c>
-      <c r="H9" s="6">
+      <c r="I35" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I9">
+      <c r="J35">
         <v>1</v>
       </c>
-      <c r="J9">
+      <c r="K35">
         <v>34</v>
       </c>
-      <c r="O9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <f>E10^$B$15*B10^$B$18*J10^$B$17*H10^$B$16*10</f>
-        <v>0.76696498884737052</v>
-      </c>
-      <c r="B10">
+    </row>
+    <row r="36" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <f>G36</f>
+        <v>-0.05</v>
+      </c>
+      <c r="C36">
         <v>75</v>
       </c>
-      <c r="C10" s="4">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="D10" s="5">
-        <f>B10/C10</f>
-        <v>7.7319587628865989</v>
-      </c>
-      <c r="E10" s="2">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G10">
+      <c r="D36" s="4">
+        <v>3.72</v>
+      </c>
+      <c r="E36" s="5">
+        <f>C36/D36</f>
+        <v>20.161290322580644</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G36" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="H36">
         <v>0.19</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I36" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <f>G37</f>
+        <v>-0.1</v>
+      </c>
+      <c r="C37">
+        <v>75</v>
+      </c>
+      <c r="D37" s="4">
+        <v>6.05</v>
+      </c>
+      <c r="E37" s="5">
+        <f>C37/D37</f>
+        <v>12.396694214876034</v>
+      </c>
+      <c r="F37" s="2">
         <v>1E-3</v>
       </c>
-      <c r="I10">
+      <c r="G37" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="H37">
+        <v>0.19</v>
+      </c>
+      <c r="I37" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J37">
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="K37">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <f>E11^$B$15*B11^$B$18*J11^$B$17*H11^$B$16*10</f>
-        <v>0.76696498884737052</v>
-      </c>
-      <c r="B11">
-        <v>120</v>
-      </c>
-      <c r="C11" s="4">
-        <v>15.4</v>
-      </c>
-      <c r="D11" s="5">
-        <f>B11/C11</f>
-        <v>7.7922077922077921</v>
-      </c>
-      <c r="E11" s="2">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G11">
+    <row r="38" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <f>G38</f>
+        <v>-0.2</v>
+      </c>
+      <c r="C38">
+        <v>75</v>
+      </c>
+      <c r="D38" s="4">
+        <v>11.1</v>
+      </c>
+      <c r="E38" s="5">
+        <f>C38/D38</f>
+        <v>6.756756756756757</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G38" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="H38">
         <v>0.19</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I38" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <f>G39</f>
+        <v>-0.3</v>
+      </c>
+      <c r="C39">
+        <v>75</v>
+      </c>
+      <c r="D39" s="4">
+        <v>17</v>
+      </c>
+      <c r="E39" s="5">
+        <f>C39/D39</f>
+        <v>4.4117647058823533</v>
+      </c>
+      <c r="F39" s="2">
         <v>1E-3</v>
       </c>
-      <c r="I11">
+      <c r="G39" s="3">
+        <v>-0.3</v>
+      </c>
+      <c r="H39">
+        <v>0.19</v>
+      </c>
+      <c r="I39" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J39">
         <v>1</v>
       </c>
-      <c r="J11">
+      <c r="K39">
         <v>34</v>
       </c>
-      <c r="L11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <f>E12^$B$15*B12^$B$18*J12^$B$17*H12^$B$16*10</f>
-        <v>1.0846522890932808</v>
-      </c>
-      <c r="B12">
+    </row>
+    <row r="40" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
+        <f>G40</f>
+        <v>-0.4</v>
+      </c>
+      <c r="C40">
         <v>75</v>
       </c>
-      <c r="C12" s="4">
-        <v>6.96</v>
-      </c>
-      <c r="D12" s="5">
-        <f>B12/C12</f>
-        <v>10.775862068965518</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D40" s="4">
+        <v>24.5</v>
+      </c>
+      <c r="E40" s="5">
+        <f>C40/D40</f>
+        <v>3.0612244897959182</v>
+      </c>
+      <c r="F40" s="2">
         <v>1E-3</v>
       </c>
-      <c r="F12" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G12">
+      <c r="G40" s="3">
+        <v>-0.4</v>
+      </c>
+      <c r="H40">
         <v>0.19</v>
       </c>
-      <c r="H12" s="6">
+      <c r="I40" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I12">
+      <c r="J40">
         <v>1</v>
       </c>
-      <c r="J12">
+      <c r="K40">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <f>E13^$B$15*B13^$B$18*J13^$B$17*H13^$B$16*10</f>
-        <v>1.4142135623730949</v>
-      </c>
-      <c r="B13">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="C43">
         <v>75</v>
       </c>
-      <c r="C13" s="4">
-        <v>5.2</v>
-      </c>
-      <c r="D13" s="5">
-        <f>B13/C13</f>
-        <v>14.423076923076923</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="F43" s="2">
         <v>1E-3</v>
       </c>
-      <c r="F13" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G13">
+      <c r="G43">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="H43">
         <v>0.19</v>
       </c>
-      <c r="H13" s="6">
+      <c r="I43" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I13">
+      <c r="J43">
         <v>1</v>
       </c>
-      <c r="J13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16">
+      <c r="K43">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="C44">
+        <v>75</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G44">
+        <v>0.192</v>
+      </c>
+      <c r="H44">
+        <v>0.19</v>
+      </c>
+      <c r="I44" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+      <c r="C45">
+        <v>75</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G45" s="3">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <f>F24</f>
+      <c r="H45">
+        <v>0.19</v>
+      </c>
+      <c r="I45" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+      <c r="C46">
+        <v>75</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G46" s="3">
         <v>0.19500000000000001</v>
       </c>
-      <c r="B24">
-        <v>75</v>
-      </c>
-      <c r="C24" s="4">
-        <v>7.6</v>
-      </c>
-      <c r="D24" s="5">
-        <f>B24/C24</f>
-        <v>9.8684210526315788</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="G24">
+      <c r="H46">
         <v>0.19</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I46" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I24">
+      <c r="J46">
         <v>1</v>
       </c>
-      <c r="J24">
+      <c r="K46">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <f>F25</f>
-        <v>0.2</v>
-      </c>
-      <c r="B25">
-        <v>75</v>
-      </c>
-      <c r="C25" s="4">
-        <v>6.96</v>
-      </c>
-      <c r="D25" s="5">
-        <f>B25/C25</f>
-        <v>10.775862068965518</v>
-      </c>
-      <c r="E25" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G25">
-        <v>0.19</v>
-      </c>
-      <c r="H25" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <f>F26</f>
-        <v>0.21</v>
-      </c>
-      <c r="B26">
-        <v>75</v>
-      </c>
-      <c r="C26" s="4">
-        <v>6.7</v>
-      </c>
-      <c r="D26" s="5">
-        <f>B26/C26</f>
-        <v>11.194029850746269</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0.21</v>
-      </c>
-      <c r="G26">
-        <v>0.19</v>
-      </c>
-      <c r="H26" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <f>F27</f>
-        <v>0.22</v>
-      </c>
-      <c r="B27">
-        <v>75</v>
-      </c>
-      <c r="C27" s="4">
-        <v>6.7</v>
-      </c>
-      <c r="D27" s="5">
-        <f>B27/C27</f>
-        <v>11.194029850746269</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="G27">
-        <v>0.19</v>
-      </c>
-      <c r="H27" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <f>F28</f>
-        <v>0.23</v>
-      </c>
-      <c r="B28">
-        <v>75</v>
-      </c>
-      <c r="C28" s="4">
-        <v>7</v>
-      </c>
-      <c r="D28" s="5">
-        <f>B28/C28</f>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="E28" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0.23</v>
-      </c>
-      <c r="G28">
-        <v>0.19</v>
-      </c>
-      <c r="H28" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-      <c r="J28">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <f>F29</f>
-        <v>0.25</v>
-      </c>
-      <c r="B29">
-        <v>75</v>
-      </c>
-      <c r="C29" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="D29" s="5">
-        <f>B29/C29</f>
-        <v>10</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="G29">
-        <v>0.19</v>
-      </c>
-      <c r="H29" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="J29">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <f>F30</f>
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="B30">
-        <v>75</v>
-      </c>
-      <c r="C30" s="4">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="D30" s="5">
-        <f>B30/C30</f>
-        <v>9.1463414634146343</v>
-      </c>
-      <c r="E30" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G30">
-        <v>0.19</v>
-      </c>
-      <c r="H30" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-      <c r="J30">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <f>F31</f>
-        <v>0.3</v>
-      </c>
-      <c r="B31">
-        <v>75</v>
-      </c>
-      <c r="C31" s="4">
-        <v>8.9</v>
-      </c>
-      <c r="D31" s="5">
-        <f>B31/C31</f>
-        <v>8.4269662921348303</v>
-      </c>
-      <c r="E31" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="G31">
-        <v>0.19</v>
-      </c>
-      <c r="H31" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-      <c r="J31">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>75</v>
-      </c>
-      <c r="E37" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F37">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="G37">
-        <v>0.19</v>
-      </c>
-      <c r="H37" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I37">
-        <v>1</v>
-      </c>
-      <c r="J37">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38">
-        <v>75</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F38">
-        <v>0.192</v>
-      </c>
-      <c r="G38">
-        <v>0.19</v>
-      </c>
-      <c r="H38" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="I38">
-        <v>1</v>
-      </c>
-      <c r="J38">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O13">
-    <sortCondition ref="A3:A13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:P40">
+    <sortCondition descending="1" ref="B23:B40"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
working on an image of the model
</commit_message>
<xml_diff>
--- a/nesh/lambda calculations.xlsx
+++ b/nesh/lambda calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nesh/Documents/Repositories/icecontinuum/nesh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C6CC21-4D7C-3F4B-9F02-0332A87243B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A09D8F-73AE-6B4A-A11F-C7ABE610944A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="15480" xr2:uid="{2DDA9610-AECA-0C43-BEDC-9A13351D73ED}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>D (um^2/us)</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>LSODA integrator, dx=.3 um</t>
+  </si>
+  <si>
+    <t>I think this is borderline stable/unstable -- the lambda is lower than the value at sigmaIcorner = 0.21, which bucks the trend</t>
   </si>
 </sst>
 </file>
@@ -612,10 +615,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$23:$B$40</c:f>
+              <c:f>Sheet1!$B$23:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.9</c:v>
                 </c:pt>
@@ -644,30 +647,27 @@
                   <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2</c:v>
+                  <c:v>-0.01</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.01</c:v>
+                  <c:v>-0.02</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.02</c:v>
+                  <c:v>-0.03</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.03</c:v>
+                  <c:v>-0.05</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.05</c:v>
+                  <c:v>-0.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.1</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.2</c:v>
+                  <c:v>-0.3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.3</c:v>
-                </c:pt>
-                <c:pt idx="17">
                   <c:v>-0.4</c:v>
                 </c:pt>
               </c:numCache>
@@ -675,10 +675,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$23:$E$40</c:f>
+              <c:f>Sheet1!$E$23:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>2.7075812274368234</c:v>
                 </c:pt>
@@ -707,30 +707,27 @@
                   <c:v>11.261261261261261</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.85383502170767</c:v>
+                  <c:v>44.117647058823529</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44.117647058823529</c:v>
+                  <c:v>33.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33.333333333333336</c:v>
+                  <c:v>27.075812274368232</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.075812274368232</c:v>
+                  <c:v>20.161290322580644</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.161290322580644</c:v>
+                  <c:v>12.396694214876034</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.396694214876034</c:v>
+                  <c:v>6.756756756756757</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.756756756756757</c:v>
+                  <c:v>4.4117647058823533</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.4117647058823533</c:v>
-                </c:pt>
-                <c:pt idx="17">
                   <c:v>3.0612244897959182</c:v>
                 </c:pt>
               </c:numCache>
@@ -2093,7 +2090,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2423,7 +2420,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="119" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomLeft" activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3219,23 +3216,23 @@
     <row r="32" spans="2:11" ht="17" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <f>G32</f>
-        <v>0.2</v>
+        <v>-0.01</v>
       </c>
       <c r="C32">
         <v>75</v>
       </c>
       <c r="D32" s="4">
-        <v>6.91</v>
+        <v>1.7</v>
       </c>
       <c r="E32" s="5">
         <f>C32/D32</f>
-        <v>10.85383502170767</v>
+        <v>44.117647058823529</v>
       </c>
       <c r="F32" s="2">
         <v>1E-3</v>
       </c>
       <c r="G32" s="3">
-        <v>0.2</v>
+        <v>-0.01</v>
       </c>
       <c r="H32">
         <v>0.19</v>
@@ -3250,26 +3247,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="17" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <f>G33</f>
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="C33">
         <v>75</v>
       </c>
       <c r="D33" s="4">
-        <v>1.7</v>
+        <v>2.25</v>
       </c>
       <c r="E33" s="5">
         <f>C33/D33</f>
-        <v>44.117647058823529</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="F33" s="2">
         <v>1E-3</v>
       </c>
       <c r="G33" s="3">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="H33">
         <v>0.19</v>
@@ -3284,26 +3281,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="17" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <f>G34</f>
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="C34">
         <v>75</v>
       </c>
       <c r="D34" s="4">
-        <v>2.25</v>
+        <v>2.77</v>
       </c>
       <c r="E34" s="5">
         <f>C34/D34</f>
-        <v>33.333333333333336</v>
+        <v>27.075812274368232</v>
       </c>
       <c r="F34" s="2">
         <v>1E-3</v>
       </c>
       <c r="G34" s="3">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="H34">
         <v>0.19</v>
@@ -3318,26 +3315,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" ht="17" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <f>G35</f>
-        <v>-0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="C35">
         <v>75</v>
       </c>
       <c r="D35" s="4">
-        <v>2.77</v>
+        <v>3.72</v>
       </c>
       <c r="E35" s="5">
         <f>C35/D35</f>
-        <v>27.075812274368232</v>
+        <v>20.161290322580644</v>
       </c>
       <c r="F35" s="2">
         <v>1E-3</v>
       </c>
       <c r="G35" s="3">
-        <v>-0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="H35">
         <v>0.19</v>
@@ -3352,26 +3349,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="17" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
         <f>G36</f>
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="C36">
         <v>75</v>
       </c>
       <c r="D36" s="4">
-        <v>3.72</v>
+        <v>6.05</v>
       </c>
       <c r="E36" s="5">
         <f>C36/D36</f>
-        <v>20.161290322580644</v>
+        <v>12.396694214876034</v>
       </c>
       <c r="F36" s="2">
         <v>1E-3</v>
       </c>
       <c r="G36" s="3">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="H36">
         <v>0.19</v>
@@ -3386,26 +3383,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="17" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
         <f>G37</f>
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="C37">
         <v>75</v>
       </c>
       <c r="D37" s="4">
-        <v>6.05</v>
+        <v>11.1</v>
       </c>
       <c r="E37" s="5">
         <f>C37/D37</f>
-        <v>12.396694214876034</v>
+        <v>6.756756756756757</v>
       </c>
       <c r="F37" s="2">
         <v>1E-3</v>
       </c>
       <c r="G37" s="3">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="H37">
         <v>0.19</v>
@@ -3420,26 +3417,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" ht="17" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
         <f>G38</f>
-        <v>-0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="C38">
         <v>75</v>
       </c>
       <c r="D38" s="4">
-        <v>11.1</v>
+        <v>17</v>
       </c>
       <c r="E38" s="5">
         <f>C38/D38</f>
-        <v>6.756756756756757</v>
+        <v>4.4117647058823533</v>
       </c>
       <c r="F38" s="2">
         <v>1E-3</v>
       </c>
       <c r="G38" s="3">
-        <v>-0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="H38">
         <v>0.19</v>
@@ -3454,26 +3451,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" ht="17" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
         <f>G39</f>
-        <v>-0.3</v>
+        <v>-0.4</v>
       </c>
       <c r="C39">
         <v>75</v>
       </c>
       <c r="D39" s="4">
-        <v>17</v>
+        <v>24.5</v>
       </c>
       <c r="E39" s="5">
         <f>C39/D39</f>
-        <v>4.4117647058823533</v>
+        <v>3.0612244897959182</v>
       </c>
       <c r="F39" s="2">
         <v>1E-3</v>
       </c>
       <c r="G39" s="3">
-        <v>-0.3</v>
+        <v>-0.4</v>
       </c>
       <c r="H39">
         <v>0.19</v>
@@ -3488,46 +3485,36 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="17" x14ac:dyDescent="0.25">
-      <c r="B40" s="3">
-        <f>G40</f>
-        <v>-0.4</v>
-      </c>
-      <c r="C40">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="C42">
         <v>75</v>
       </c>
-      <c r="D40" s="4">
-        <v>24.5</v>
-      </c>
-      <c r="E40" s="5">
-        <f>C40/D40</f>
-        <v>3.0612244897959182</v>
-      </c>
-      <c r="F40" s="2">
+      <c r="F42" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G40" s="3">
-        <v>-0.4</v>
-      </c>
-      <c r="H40">
+      <c r="G42">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="H42">
         <v>0.19</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I42" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J40">
+      <c r="J42">
         <v>1</v>
       </c>
-      <c r="K40">
+      <c r="K42">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
       <c r="C43">
         <v>75</v>
       </c>
@@ -3535,7 +3522,7 @@
         <v>1E-3</v>
       </c>
       <c r="G43">
-        <v>0.19400000000000001</v>
+        <v>0.192</v>
       </c>
       <c r="H43">
         <v>0.19</v>
@@ -3550,16 +3537,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="17" x14ac:dyDescent="0.25">
-      <c r="B44" s="5"/>
+    <row r="44" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
       <c r="C44">
         <v>75</v>
       </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="5"/>
       <c r="F44" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G44">
-        <v>0.192</v>
+      <c r="G44" s="3">
+        <v>-0.5</v>
       </c>
       <c r="H44">
         <v>0.19</v>
@@ -3574,7 +3563,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" ht="17" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
       <c r="C45">
         <v>75</v>
@@ -3585,7 +3574,7 @@
         <v>1E-3</v>
       </c>
       <c r="G45" s="3">
-        <v>-0.5</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="H45">
         <v>0.19</v>
@@ -3600,18 +3589,23 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="17" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
       <c r="C46">
         <v>75</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="5"/>
+      <c r="D46" s="4">
+        <v>6.91</v>
+      </c>
+      <c r="E46" s="5">
+        <f>C46/D46</f>
+        <v>10.85383502170767</v>
+      </c>
       <c r="F46" s="2">
         <v>1E-3</v>
       </c>
       <c r="G46" s="3">
-        <v>0.19500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="H46">
         <v>0.19</v>
@@ -3625,10 +3619,13 @@
       <c r="K46">
         <v>34</v>
       </c>
+      <c r="L46" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:P40">
-    <sortCondition descending="1" ref="B23:B40"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:P39">
+    <sortCondition descending="1" ref="B23:B39"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Working on figures for the paper
</commit_message>
<xml_diff>
--- a/nesh/lambda calculations.xlsx
+++ b/nesh/lambda calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nesh/Documents/Repositories/icecontinuum/nesh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A09D8F-73AE-6B4A-A11F-C7ABE610944A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9621D3-9ABC-F543-85BC-3AE1776D2A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="15480" xr2:uid="{2DDA9610-AECA-0C43-BEDC-9A13351D73ED}"/>
   </bookViews>
@@ -292,7 +292,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.32659863237109038</c:v>
@@ -334,7 +334,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$2:$E$12</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>3.0120481927710845</c:v>
@@ -412,7 +412,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -475,7 +475,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -701,7 +701,7 @@
                   <c:v>10.714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.194029850746269</c:v>
+                  <c:v>11.061946902654867</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>11.261261261261261</c:v>
@@ -710,7 +710,7 @@
                   <c:v>44.117647058823529</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.333333333333336</c:v>
+                  <c:v>33.185840707964601</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>27.075812274368232</c:v>
@@ -2082,16 +2082,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>21345</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>74706</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2418,9 +2418,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FACA8F-BEA8-A344-9B24-B4206D9D79F6}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="119" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2472,7 +2472,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <f>F2^$C$14*C2^$C$17*K2^$C$16*I2^$C$15*10</f>
         <v>0.32659863237109038</v>
       </c>
@@ -2482,7 +2482,7 @@
       <c r="D2" s="4">
         <v>24.9</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <f>C2/D2</f>
         <v>3.0120481927710845</v>
       </c>
@@ -2506,8 +2506,8 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B3" s="4">
-        <f>F3^$C$14*C3^$C$17*K3^$C$16*I3^$C$15*10</f>
+      <c r="B3" s="3">
+        <f t="shared" ref="B3:B12" si="0">F3^$C$14*C3^$C$17*K3^$C$16*I3^$C$15*10</f>
         <v>0.34299717028501764</v>
       </c>
       <c r="C3">
@@ -2516,7 +2516,7 @@
       <c r="D3" s="4">
         <v>22.9</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <f>C3/D3</f>
         <v>3.2751091703056772</v>
       </c>
@@ -2540,8 +2540,8 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B4" s="4">
-        <f>F4^$C$14*C4^$C$17*K4^$C$16*I4^$C$15*10</f>
+      <c r="B4" s="3">
+        <f t="shared" si="0"/>
         <v>0.34299717028501764</v>
       </c>
       <c r="C4">
@@ -2550,7 +2550,7 @@
       <c r="D4" s="4">
         <v>22.5</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <f>C4/D4</f>
         <v>3.3333333333333335</v>
       </c>
@@ -2574,8 +2574,8 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B5" s="4">
-        <f>F5^$C$14*C5^$C$17*K5^$C$16*I5^$C$15*10</f>
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
         <v>0.48507125007266588</v>
       </c>
       <c r="C5">
@@ -2584,7 +2584,7 @@
       <c r="D5" s="4">
         <v>16</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <f>C5/D5</f>
         <v>4.6875</v>
       </c>
@@ -2611,8 +2611,8 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B6" s="4">
-        <f>F6^$C$14*C6^$C$17*K6^$C$16*I6^$C$15*10</f>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
         <v>0.48507125007266588</v>
       </c>
       <c r="C6">
@@ -2621,7 +2621,7 @@
       <c r="D6" s="4">
         <v>15.4</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <f>C6/D6</f>
         <v>4.8701298701298699</v>
       </c>
@@ -2645,8 +2645,8 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
-        <f>F7^$C$14*C7^$C$17*K7^$C$16*I7^$C$15*10</f>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
         <v>0.48507125007266588</v>
       </c>
       <c r="C7">
@@ -2655,7 +2655,7 @@
       <c r="D7" s="4">
         <v>14.8</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f>C7/D7</f>
         <v>5.0675675675675675</v>
       </c>
@@ -2682,8 +2682,8 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
-        <f>F8^$C$14*C8^$C$17*K8^$C$16*I8^$C$15*10</f>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
         <v>0.76696498884737041</v>
       </c>
       <c r="C8">
@@ -2692,7 +2692,7 @@
       <c r="D8" s="4">
         <v>10</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f>C8/D8</f>
         <v>7.5</v>
       </c>
@@ -2719,8 +2719,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
-        <f>F9^$C$14*C9^$C$17*K9^$C$16*I9^$C$15*10</f>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
         <v>0.76696498884737052</v>
       </c>
       <c r="C9">
@@ -2729,7 +2729,7 @@
       <c r="D9" s="4">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <f>C9/D9</f>
         <v>7.7319587628865989</v>
       </c>
@@ -2753,8 +2753,8 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
-        <f>F10^$C$14*C10^$C$17*K10^$C$16*I10^$C$15*10</f>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
         <v>0.76696498884737052</v>
       </c>
       <c r="C10">
@@ -2763,7 +2763,7 @@
       <c r="D10" s="4">
         <v>15.4</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f>C10/D10</f>
         <v>7.7922077922077921</v>
       </c>
@@ -2790,8 +2790,8 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <f>F11^$C$14*C11^$C$17*K11^$C$16*I11^$C$15*10</f>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
         <v>1.0846522890932808</v>
       </c>
       <c r="C11">
@@ -2800,7 +2800,7 @@
       <c r="D11" s="4">
         <v>6.96</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <f>C11/D11</f>
         <v>10.775862068965518</v>
       </c>
@@ -2824,8 +2824,8 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
-        <f>F12^$C$14*C12^$C$17*K12^$C$16*I12^$C$15*10</f>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
         <v>1.4142135623730949</v>
       </c>
       <c r="C12">
@@ -2834,7 +2834,7 @@
       <c r="D12" s="4">
         <v>5.2</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <f>C12/D12</f>
         <v>14.423076923076923</v>
       </c>
@@ -3154,11 +3154,11 @@
         <v>75</v>
       </c>
       <c r="D30" s="4">
-        <v>6.7</v>
+        <v>6.78</v>
       </c>
       <c r="E30" s="5">
         <f>C30/D30</f>
-        <v>11.194029850746269</v>
+        <v>11.061946902654867</v>
       </c>
       <c r="F30" s="2">
         <v>1E-3</v>
@@ -3256,11 +3256,11 @@
         <v>75</v>
       </c>
       <c r="D33" s="4">
-        <v>2.25</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="E33" s="5">
         <f>C33/D33</f>
-        <v>33.333333333333336</v>
+        <v>33.185840707964601</v>
       </c>
       <c r="F33" s="2">
         <v>1E-3</v>

</xml_diff>